<commit_message>
union casos de uso
</commit_message>
<xml_diff>
--- a/trunk/docs/Entregables/ERRORES 27.10.2016.xlsx
+++ b/trunk/docs/Entregables/ERRORES 27.10.2016.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>Usuario</t>
   </si>
@@ -71,31 +71,6 @@
     <t>No se elimina el tema, salta un mensaje "No se pudo eliminar el tema"</t>
   </si>
   <si>
-    <t>ADMIN</t>
-  </si>
-  <si>
-    <t>Crear alumno</t>
-  </si>
-  <si>
-    <t>No ser pudo guardar alumno
-Legajo:
-123123
-Nombre:
-123123
-Apellido:
-123
-Tipo de Documento:
-123
-Número de Documento:
-123
-Género:
-Email:
-123@123
-SEGURIDAD
-Nombre de Usuario:
-123</t>
-  </si>
-  <si>
     <t>agregar actividades a un concepto deshabilitado</t>
   </si>
   <si>
@@ -112,6 +87,39 @@
   </si>
   <si>
     <t>editar actividad</t>
+  </si>
+  <si>
+    <t>cuando el tema está eliminado no deberia aparecer para poder elegirse como predecesor.</t>
+  </si>
+  <si>
+    <t>docente</t>
+  </si>
+  <si>
+    <t>Seleccionar predecesora</t>
+  </si>
+  <si>
+    <t>Selección que quede encolumnada</t>
+  </si>
+  <si>
+    <t>alumno</t>
+  </si>
+  <si>
+    <t>renovar contraseña</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no se renueva la contraseña desde el admin </t>
+  </si>
+  <si>
+    <t>boton volver</t>
+  </si>
+  <si>
+    <t>cambiar el boton volver de temas y conceptos cambiar la posición del mismo arriba a la derecha</t>
+  </si>
+  <si>
+    <t>carga y modificacion de temas y conceptos</t>
+  </si>
+  <si>
+    <t>Estan invertidos los campos copete y descripción</t>
   </si>
 </sst>
 </file>
@@ -498,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,27 +597,27 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" ht="255" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2"/>
     </row>
@@ -618,7 +626,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>19</v>
@@ -630,35 +638,59 @@
         <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -883,12 +915,6 @@
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modificacion de casos de uso del incremento 2
</commit_message>
<xml_diff>
--- a/trunk/docs/Entregables/ERRORES 27.10.2016.xlsx
+++ b/trunk/docs/Entregables/ERRORES 27.10.2016.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>Usuario</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Estan invertidos los campos copete y descripción</t>
+  </si>
+  <si>
+    <t>blanqueo de sucesoras</t>
   </si>
 </sst>
 </file>
@@ -509,7 +512,7 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,9 +697,13 @@
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ajustes a los documentos
</commit_message>
<xml_diff>
--- a/trunk/docs/Entregables/ERRORES 27.10.2016.xlsx
+++ b/trunk/docs/Entregables/ERRORES 27.10.2016.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t>Usuario</t>
   </si>
@@ -123,6 +124,15 @@
   </si>
   <si>
     <t>blanqueo de sucesoras</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>en proceso</t>
   </si>
 </sst>
 </file>
@@ -160,7 +170,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -183,16 +193,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -509,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,7 +561,7 @@
     <col min="4" max="4" width="70" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -535,8 +574,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -549,8 +591,11 @@
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E2" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -563,8 +608,11 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -575,8 +623,11 @@
         <v>11</v>
       </c>
       <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -587,8 +638,11 @@
         <v>12</v>
       </c>
       <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -599,8 +653,11 @@
         <v>14</v>
       </c>
       <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E6" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -611,8 +668,11 @@
         <v>15</v>
       </c>
       <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -623,8 +683,11 @@
         <v>16</v>
       </c>
       <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -635,8 +698,11 @@
         <v>19</v>
       </c>
       <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -647,8 +713,11 @@
         <v>21</v>
       </c>
       <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E10" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -659,8 +728,11 @@
         <v>24</v>
       </c>
       <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E11" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -672,7 +744,7 @@
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
@@ -684,7 +756,7 @@
       </c>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -695,8 +767,11 @@
         <v>31</v>
       </c>
       <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -705,8 +780,11 @@
         <v>32</v>
       </c>
       <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>

</xml_diff>